<commit_message>
edit the old file
</commit_message>
<xml_diff>
--- a/admin_panel/push_management/push_message.xlsx
+++ b/admin_panel/push_management/push_message.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\admin_panel\push_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56879207-5151-446B-8FF1-D9C0C767FBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4FA8F1-D294-4FC8-BB6E-44A0E0062FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="83">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -49,121 +49,46 @@
     <t>Expected result</t>
   </si>
   <si>
-    <t>check with empty text in the template name field</t>
-  </si>
-  <si>
-    <t>enter a valid and unique template name.</t>
-  </si>
-  <si>
     <t>an error message will show " This field is required."</t>
-  </si>
-  <si>
-    <t>enter the minimum allowed characters into the input text field.</t>
   </si>
   <si>
     <t>****</t>
   </si>
   <si>
-    <t>the input is accepted, and no error message is displayed.</t>
-  </si>
-  <si>
     <t>the form is submitted successfully</t>
-  </si>
-  <si>
-    <t>enter only alphabetic characters into the input text field.</t>
   </si>
   <si>
     <t>the input is accepted without any issues.</t>
   </si>
   <si>
-    <t>enter numeric characters into the input text field.</t>
-  </si>
-  <si>
-    <t>enter a combination of alphabetic and numeric characters.</t>
-  </si>
-  <si>
-    <t>enter special characters into the input text field.</t>
-  </si>
-  <si>
     <t>the input is accepted if special characters are allowed; otherwise, an error is displayed.</t>
-  </si>
-  <si>
-    <t>enter text with leading whitespaces.</t>
   </si>
   <si>
     <t>the input is accepted, and leading whitespaces are trimmed.</t>
   </si>
   <si>
-    <t>enter text with trailing whitespaces.</t>
-  </si>
-  <si>
-    <t>enter text with spaces within the content.</t>
-  </si>
-  <si>
-    <t>enter text in uppercase letters.</t>
-  </si>
-  <si>
-    <t>enter text in lowercase letters.</t>
-  </si>
-  <si>
-    <t>enter text with a mix of uppercase and lowercase letters.</t>
-  </si>
-  <si>
-    <t>enter text with punctuation marks.</t>
-  </si>
-  <si>
     <t>the input is accepted if punctuation marks are allowed; otherwise, an error is displayed</t>
-  </si>
-  <si>
-    <t>enter text with line breaks or newlines.</t>
   </si>
   <si>
     <t>the input is accepted without issues; newline characters are handled appropriately.</t>
   </si>
   <si>
-    <t>attempt to inject HTML or script tags into the input text field.</t>
-  </si>
-  <si>
     <t>the input is rejected, and an error message is displayed.</t>
-  </si>
-  <si>
-    <t>enter text containing emojis.</t>
   </si>
   <si>
     <t>the input is accepted if emojis are allowed; otherwise, an error is displayed.</t>
   </si>
   <si>
-    <t>enter text with accented characters (e.g., é, ü).</t>
-  </si>
-  <si>
-    <t>enter the default placeholder text into the input field.</t>
-  </si>
-  <si>
     <t>the placeholder text disappears when the user starts typing, and the input is accepted.</t>
   </si>
   <si>
-    <t>enter text, then clear the input text field.</t>
-  </si>
-  <si>
     <t>the input is cleared, and the field becomes empty.</t>
-  </si>
-  <si>
-    <t>enter text, then undo the input action.</t>
   </si>
   <si>
     <t>the input is undone, and the field reverts to its previous state.</t>
   </si>
   <si>
     <t>the user is on the "add push template form" page.</t>
-  </si>
-  <si>
-    <t>enter text, undo, then redo the input action.</t>
-  </si>
-  <si>
-    <t>paste text into the input text field using the paste action.</t>
-  </si>
-  <si>
-    <t>copy and cut text from the input text field.</t>
   </si>
   <si>
     <t>the input is redone, and the field returns to the modified state.</t>
@@ -176,15 +101,6 @@
   </si>
   <si>
     <t>the copied/cut text is successfully performed, and the input is modified accordingly.</t>
-  </si>
-  <si>
-    <t>enter text and navigate through the input field using the tab key.</t>
-  </si>
-  <si>
-    <t>enter the maximum allowed characters into the input text field.(more than 100 characters)</t>
-  </si>
-  <si>
-    <t>an error message will show "please enter no more than 100 characters."</t>
   </si>
   <si>
     <t>Test Scenario: Push Message</t>
@@ -274,6 +190,90 @@
 4. go to push template
 5. go to add new template
 6. try to check with empty text in the message field</t>
+  </si>
+  <si>
+    <t>check with empty text in the message field</t>
+  </si>
+  <si>
+    <t>an error message will show "Please enter no more than 250 characters."</t>
+  </si>
+  <si>
+    <t>an error message will show,"Please enter at least 10 characters."</t>
+  </si>
+  <si>
+    <t>enter a valid and unique message</t>
+  </si>
+  <si>
+    <t>enter the maximum number of allowed characters into the  message field. (more than 250 characters)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enter the minimum number of allowed characters into the message field. (less than 10 characters). </t>
+  </si>
+  <si>
+    <t>enter only alphabetic characters into the message field field.</t>
+  </si>
+  <si>
+    <t>enter numeric characters into the message field.</t>
+  </si>
+  <si>
+    <t>enter a combination of alphabetic and numeric characters into the message field.</t>
+  </si>
+  <si>
+    <t>enter special characters into the message field.</t>
+  </si>
+  <si>
+    <t>enter text with leading whitespacesinto the message field.</t>
+  </si>
+  <si>
+    <t>enter text with trailing whitespaces into the message field.</t>
+  </si>
+  <si>
+    <t>enter text with spaces within the content into the message field.</t>
+  </si>
+  <si>
+    <t>enter text in uppercase letters into the message field.</t>
+  </si>
+  <si>
+    <t>enter text in lowercase letters into the message field.</t>
+  </si>
+  <si>
+    <t>enter text with a mix of uppercase and lowercase letters into the message field.</t>
+  </si>
+  <si>
+    <t>enter text with punctuation marks into the message field.</t>
+  </si>
+  <si>
+    <t>enter text with line breaks or newlines into the message field.</t>
+  </si>
+  <si>
+    <t>attempt to inject HTML or script tags into the message field.</t>
+  </si>
+  <si>
+    <t>enter text containing emojis into the message field.</t>
+  </si>
+  <si>
+    <t>enter text with accented characters (e.g., é, ü) into the message field.</t>
+  </si>
+  <si>
+    <t>enter the default placeholder text into the message field.</t>
+  </si>
+  <si>
+    <t>enter text, then clear  the message field.</t>
+  </si>
+  <si>
+    <t>enter text, then undo  the message field.</t>
+  </si>
+  <si>
+    <t>enter text, undo, and then redo the message field.</t>
+  </si>
+  <si>
+    <t>enter text and navigate through the message field using the tab key.</t>
+  </si>
+  <si>
+    <t>paste the text into the message field using the paste action.</t>
+  </si>
+  <si>
+    <t>copy and cut text from  the message field.</t>
   </si>
 </sst>
 </file>
@@ -1369,15 +1369,15 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G2"/>
+      <pane ySplit="3" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.109375" style="15" customWidth="1"/>
     <col min="2" max="2" width="21.109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="44.44140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" style="20" customWidth="1"/>
     <col min="4" max="4" width="57.33203125" style="18" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" style="20" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="21" customWidth="1"/>
@@ -1387,7 +1387,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -1487,19 +1487,19 @@
     </row>
     <row r="4" spans="1:26" ht="120" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>6</v>
@@ -1529,19 +1529,19 @@
     </row>
     <row r="5" spans="1:26" ht="123" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>13</v>
-      </c>
       <c r="E5" s="10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -1567,19 +1567,19 @@
     </row>
     <row r="6" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1605,19 +1605,19 @@
     </row>
     <row r="7" spans="1:26" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1643,19 +1643,19 @@
     </row>
     <row r="8" spans="1:26" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1681,19 +1681,19 @@
     </row>
     <row r="9" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
@@ -1719,19 +1719,19 @@
     </row>
     <row r="10" spans="1:26" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
@@ -1757,19 +1757,19 @@
     </row>
     <row r="11" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="8"/>
@@ -1795,19 +1795,19 @@
     </row>
     <row r="12" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="8"/>
@@ -1833,19 +1833,19 @@
     </row>
     <row r="13" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="8"/>
@@ -1871,19 +1871,19 @@
     </row>
     <row r="14" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F14" s="6"/>
       <c r="G14" s="8"/>
@@ -1909,19 +1909,19 @@
     </row>
     <row r="15" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="8"/>
@@ -1947,19 +1947,19 @@
     </row>
     <row r="16" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="8"/>
@@ -1985,19 +1985,19 @@
     </row>
     <row r="17" spans="1:26" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="8"/>
@@ -2023,19 +2023,19 @@
     </row>
     <row r="18" spans="1:26" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="8"/>
@@ -2061,19 +2061,19 @@
     </row>
     <row r="19" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="8"/>
@@ -2099,19 +2099,19 @@
     </row>
     <row r="20" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="8"/>
@@ -2137,19 +2137,19 @@
     </row>
     <row r="21" spans="1:26" ht="87.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="8"/>
@@ -2175,19 +2175,19 @@
     </row>
     <row r="22" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="8"/>
@@ -2213,19 +2213,19 @@
     </row>
     <row r="23" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="8"/>
@@ -2251,19 +2251,19 @@
     </row>
     <row r="24" spans="1:26" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="8"/>
@@ -2289,19 +2289,19 @@
     </row>
     <row r="25" spans="1:26" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
@@ -2327,19 +2327,19 @@
     </row>
     <row r="26" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="9"/>
@@ -2365,19 +2365,19 @@
     </row>
     <row r="27" spans="1:26" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F27" s="6"/>
       <c r="G27" s="9"/>
@@ -2403,19 +2403,19 @@
     </row>
     <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>46</v>
+        <v>81</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="9"/>
@@ -2441,19 +2441,19 @@
     </row>
     <row r="29" spans="1:26" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="9"/>

</xml_diff>